<commit_message>
bug fixes and check vals from spreadsheet
</commit_message>
<xml_diff>
--- a/Data/fracnonstrpanels.xlsx
+++ b/Data/fracnonstrpanels.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1740" windowWidth="26680" windowHeight="13200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -351,7 +351,7 @@
   <dimension ref="A1:S151"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>